<commit_message>
Re-Avaliação GRE - EDUARDO Concluida
</commit_message>
<xml_diff>
--- a/Gerência de Requisitos/Eduardo/Planilha GRE.xlsx
+++ b/Gerência de Requisitos/Eduardo/Planilha GRE.xlsx
@@ -15,74 +15,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="D67" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Link não funciona, foi usado o link apresentado no RAP3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D88" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Link não funciona.
-Não fala nada sobre experiencias ou treinamentos dos indivíduos que executarão o processo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D95" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Link não funciona.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D102" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Esse documento não tem validade se ele não foi feito/atestado por ninguém (assinado)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>INSTRUÇÕES</t>
   </si>
@@ -157,9 +91,6 @@
     <t>(T,L,P,N,NA)</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>GRE 2. Os requisitos são avaliados com base em critérios objetivos e um comprometimento da equipe técnica com estes requisitos é obtido.
 As evidências apresentadas para este resultado permitem assegurar: (i) que foi obtido e registrado um comprometimento formal da equipe técnica com os requisitos aprovados? (ii) que foram definidos critérios para análise de requisitos e que estes foram usados como base para a avaliação e a aceitação dos requisitos do projeto (por parte da equipe técnica)? (iii) que um novo comprometimento da equipe técnica com os requisitos foi obtido e registrado quando houve mudanças nos requisitos?</t>
   </si>
@@ -222,7 +153,10 @@
     <t>Plano de Monitoramento do Cronograma</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Definição do Processo de Gerência de Requisitos</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
   <si>
     <t>AP 2.1 O processo é gerenciado</t>
@@ -245,6 +179,9 @@
     <t>RAP 4. (Para o nível G). A execução do processo é monitorada e ajustes são realizados.                                                                                As evidências apresentadas para este resultado permitem assegurar que  o processo foi executado conforme planejado e que ações corretivas foram tomadas quando a execução do processo se desviou dos planos?</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>RAP 5. As informações e os recursos necessários para a execução do processo são identificados e disponibilizados.
 As evidências apresentadas para este resultado permitem assegurar que foram identificados e disponibilizados os recursos necessários (ex: pessoal, financeiros,hardware/infra-estrutura, software/ferramentas) e as informações necessárias (ex: processos, padrões, modelos, guias) para executar o processo?</t>
   </si>
@@ -274,14 +211,14 @@
     <t>Documento de Auditoria de Qualidade</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>RAP 10. (Para o nível G). O processo planejado para o projeto é executado.                                                                           
 As evidências apresentadas para este resultado permitem assegurar que o projeto foi conduzido a partir da execução do seu processo planejado, bem como se existem registros de execução das atividades do processo com base no seu planejamento?</t>
   </si>
   <si>
     <t>Documento de acompanhamento de não-conformidades</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
 </sst>
 </file>
@@ -381,6 +318,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -422,12 +366,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -468,8 +406,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF3333"/>
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -480,8 +418,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3333"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFCF305"/>
       </patternFill>
     </fill>
   </fills>
@@ -704,7 +642,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -817,7 +755,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,11 +775,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -873,11 +807,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -885,11 +819,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -897,11 +831,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -913,11 +847,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -925,7 +859,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -933,15 +867,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -949,31 +891,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="16" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -995,10 +937,10 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFCF305"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1019,7 +961,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFCF305"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -1038,7 +980,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1067,10 +1009,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="160.857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="3" style="0" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="157.265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1458,16 +1400,17 @@
   </sheetPr>
   <dimension ref="A1:Z114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D115" activeCellId="0" sqref="D115"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="3.28571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="3.23979591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,7 +1473,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
@@ -1568,7 +1511,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -1788,9 +1731,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="31"/>
-      <c r="D11" s="31" t="s">
-        <v>24</v>
-      </c>
+      <c r="D11" s="31"/>
       <c r="E11" s="32"/>
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
@@ -1816,7 +1757,7 @@
     </row>
     <row r="12" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="24"/>
@@ -1846,7 +1787,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="27" t="str">
@@ -1881,14 +1822,14 @@
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Crit%C3%A9rios%20para%20Analise%20de%20Requisitos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="26"/>
@@ -1916,14 +1857,14 @@
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="26"/>
@@ -1951,14 +1892,14 @@
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="26"/>
@@ -1986,14 +1927,14 @@
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="26"/>
@@ -2051,7 +1992,7 @@
     </row>
     <row r="19" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -2081,14 +2022,14 @@
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Ger%C3%AAncia%20de%20Requisitos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="26"/>
@@ -2258,7 +2199,7 @@
     </row>
     <row r="26" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
@@ -2288,14 +2229,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Revis%C3%A3o%20de%20Requisito.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="26"/>
@@ -2323,14 +2264,14 @@
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Revis%C3%A3o%20de%20Requisito.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="26"/>
@@ -2472,7 +2413,7 @@
     </row>
     <row r="33" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2502,14 +2443,14 @@
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="26"/>
@@ -2537,14 +2478,14 @@
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="26"/>
@@ -2572,14 +2513,14 @@
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="27" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GRE/Documento%20de%20Registro%20de%20Mudan%C3%A7a.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E36" s="26"/>
@@ -2662,13 +2603,13 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="1"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -2692,11 +2633,11 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
       <c r="F40" s="1"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -2720,13 +2661,13 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
+      <c r="A41" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="42"/>
       <c r="F41" s="1"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2750,13 +2691,13 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="45"/>
       <c r="F42" s="1"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2780,13 +2721,13 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="50"/>
+      <c r="A43" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="47"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49"/>
       <c r="F43" s="1"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2810,13 +2751,13 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="54"/>
+      <c r="A44" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="51"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="53"/>
       <c r="F44" s="1"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2841,14 +2782,14 @@
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="26"/>
-      <c r="C45" s="55" t="str">
+      <c r="C45" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Monitoramento%20do%20Cronograma.xlsx","X")</f>
         <v>X</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D45" s="55" t="s">
         <v>21</v>
       </c>
       <c r="E45" s="26"/>
@@ -2874,11 +2815,15 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="25"/>
+    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="B46" s="26"/>
       <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
+      <c r="D46" s="56" t="s">
+        <v>21</v>
+      </c>
       <c r="E46" s="26"/>
       <c r="F46" s="1"/>
       <c r="G46" s="3"/>
@@ -2966,7 +2911,7 @@
       <c r="E49" s="26"/>
       <c r="F49" s="1"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="H49" s="57"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3019,13 +2964,13 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="54"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="53"/>
       <c r="F51" s="1"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -3049,13 +2994,13 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="60" t="s">
+      <c r="A52" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="61"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="54"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="53"/>
       <c r="F52" s="1"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -3083,11 +3028,11 @@
         <v>47</v>
       </c>
       <c r="B53" s="26"/>
-      <c r="C53" s="55" t="str">
+      <c r="C53" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Projeto.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D53" s="63" t="s">
+      <c r="D53" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E53" s="26"/>
@@ -3258,13 +3203,13 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="60" t="s">
+      <c r="A59" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="64"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="54"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="53"/>
       <c r="F59" s="1"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -3289,14 +3234,14 @@
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="26"/>
-      <c r="C60" s="55" t="str">
+      <c r="C60" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Monitoramento%20do%20Cronograma.xlsx","X")</f>
         <v>X</v>
       </c>
-      <c r="D60" s="63" t="s">
+      <c r="D60" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E60" s="26"/>
@@ -3441,7 +3386,7 @@
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E65" s="32"/>
       <c r="F65" s="1"/>
@@ -3467,13 +3412,13 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="65"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="54"/>
+      <c r="B66" s="66"/>
+      <c r="C66" s="66"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="53"/>
       <c r="F66" s="1"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -3498,16 +3443,15 @@
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B67" s="26"/>
-      <c r="C67" s="55" t="str">
+      <c r="C67" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Monitoramento%20do%20Cronograma.xlsx","X")</f>
         <v>X</v>
       </c>
-      <c r="D67" s="66" t="str">
-        <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Monitoramento%20do%20Cronograma.xlsx","X")</f>
-        <v>X</v>
+      <c r="D67" s="55" t="s">
+        <v>21</v>
       </c>
       <c r="E67" s="26"/>
       <c r="F67" s="1"/>
@@ -3651,7 +3595,7 @@
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="1"/>
@@ -3676,14 +3620,14 @@
       <c r="Y72" s="3"/>
       <c r="Z72" s="3"/>
     </row>
-    <row r="73" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="B73" s="65"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="54"/>
+    <row r="73" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="53"/>
       <c r="F73" s="1"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
@@ -3708,14 +3652,14 @@
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B74" s="26"/>
-      <c r="C74" s="55" t="str">
+      <c r="C74" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Recursos%20Humanos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D74" s="63" t="s">
+      <c r="D74" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E74" s="26"/>
@@ -3746,11 +3690,11 @@
         <v>47</v>
       </c>
       <c r="B75" s="26"/>
-      <c r="C75" s="55" t="str">
+      <c r="C75" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Projeto.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D75" s="63" t="s">
+      <c r="D75" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E75" s="26"/>
@@ -3893,13 +3837,13 @@
       <c r="Z79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="B80" s="65"/>
-      <c r="C80" s="65"/>
-      <c r="D80" s="65"/>
-      <c r="E80" s="54"/>
+      <c r="A80" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="66"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="53"/>
       <c r="F80" s="1"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -3924,14 +3868,14 @@
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B81" s="26"/>
-      <c r="C81" s="55" t="str">
+      <c r="C81" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GPR/Plano%20de%20Recursos%20Humanos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D81" s="63" t="s">
+      <c r="D81" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="26"/>
@@ -4076,7 +4020,7 @@
       </c>
       <c r="C86" s="31"/>
       <c r="D86" s="31" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="1"/>
@@ -4102,13 +4046,13 @@
       <c r="Z86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="B87" s="65"/>
-      <c r="C87" s="65"/>
-      <c r="D87" s="65"/>
-      <c r="E87" s="54"/>
+      <c r="A87" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B87" s="66"/>
+      <c r="C87" s="66"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="53"/>
       <c r="F87" s="1"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -4133,16 +4077,15 @@
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B88" s="26"/>
-      <c r="C88" s="55" t="str">
+      <c r="C88" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Ger%C3%AAncia%20de%20Requisitos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D88" s="67" t="str">
-        <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Ger%C3%AAncia%20de%20Requisitos.docx","X")</f>
-        <v>X</v>
+      <c r="D88" s="67" t="s">
+        <v>21</v>
       </c>
       <c r="E88" s="26"/>
       <c r="F88" s="1"/>
@@ -4286,7 +4229,7 @@
       </c>
       <c r="C93" s="31"/>
       <c r="D93" s="31" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="1"/>
@@ -4312,13 +4255,13 @@
       <c r="Z93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="B94" s="65"/>
-      <c r="C94" s="65"/>
-      <c r="D94" s="65"/>
-      <c r="E94" s="54"/>
+      <c r="A94" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B94" s="66"/>
+      <c r="C94" s="66"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="53"/>
       <c r="F94" s="1"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -4343,16 +4286,15 @@
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B95" s="26"/>
-      <c r="C95" s="55" t="str">
+      <c r="C95" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Ger%C3%AAncia%20de%20Requisitos.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D95" s="67" t="str">
-        <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/Documento%20de%20Defini%C3%A7%C3%A3o%20de%20Processo%20de%20Ger%C3%AAncia%20de%20Requisitos.docx","X")</f>
-        <v>X</v>
+      <c r="D95" s="68" t="s">
+        <v>21</v>
       </c>
       <c r="E95" s="26"/>
       <c r="F95" s="1"/>
@@ -4496,7 +4438,7 @@
       </c>
       <c r="C100" s="31"/>
       <c r="D100" s="31" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E100" s="32"/>
       <c r="F100" s="1"/>
@@ -4522,13 +4464,13 @@
       <c r="Z100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B101" s="65"/>
-      <c r="C101" s="65"/>
-      <c r="D101" s="65"/>
-      <c r="E101" s="54"/>
+      <c r="A101" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B101" s="66"/>
+      <c r="C101" s="66"/>
+      <c r="D101" s="66"/>
+      <c r="E101" s="53"/>
       <c r="F101" s="1"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -4553,14 +4495,14 @@
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B102" s="26"/>
-      <c r="C102" s="55" t="str">
+      <c r="C102" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Documento%20de%20auditoria%20de%20qualidade.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D102" s="68" t="s">
+      <c r="D102" s="69" t="s">
         <v>21</v>
       </c>
       <c r="E102" s="26"/>
@@ -4705,7 +4647,7 @@
       </c>
       <c r="C107" s="31"/>
       <c r="D107" s="31" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E107" s="32"/>
       <c r="F107" s="1"/>
@@ -4731,13 +4673,13 @@
       <c r="Z107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B108" s="65"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="54"/>
+      <c r="A108" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B108" s="66"/>
+      <c r="C108" s="66"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="53"/>
       <c r="F108" s="1"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
@@ -4762,14 +4704,14 @@
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B109" s="26"/>
-      <c r="C109" s="55" t="str">
+      <c r="C109" s="54" t="str">
         <f aca="false">HYPERLINK("https://github.com/gilmarfilho/ProcessoDeSoftware/blob/master/TEMPLATES/TEMPLATES%20GQA/Documento%20de%20acompanhamento%20de%20n%C3%A3o-conformidades.docx","X")</f>
         <v>X</v>
       </c>
-      <c r="D109" s="63" t="s">
+      <c r="D109" s="64" t="s">
         <v>21</v>
       </c>
       <c r="E109" s="26"/>
@@ -4914,7 +4856,7 @@
       </c>
       <c r="C114" s="31"/>
       <c r="D114" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E114" s="32"/>
       <c r="F114" s="1"/>
@@ -4941,26 +4883,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId2" display="X"/>
-    <hyperlink ref="D7" r:id="rId3" display="X"/>
-    <hyperlink ref="D13" r:id="rId4" display="X"/>
-    <hyperlink ref="D14" r:id="rId5" display="X"/>
-    <hyperlink ref="D15" r:id="rId6" display="X"/>
-    <hyperlink ref="D16" r:id="rId7" display="X"/>
-    <hyperlink ref="D17" r:id="rId8" display="X"/>
+    <hyperlink ref="D6" r:id="rId1" display="X"/>
+    <hyperlink ref="D7" r:id="rId2" display="X"/>
+    <hyperlink ref="D13" r:id="rId3" display="X"/>
+    <hyperlink ref="D14" r:id="rId4" display="X"/>
+    <hyperlink ref="D15" r:id="rId5" display="X"/>
+    <hyperlink ref="D16" r:id="rId6" display="X"/>
+    <hyperlink ref="D17" r:id="rId7" display="X"/>
+    <hyperlink ref="D20" r:id="rId8" display="X"/>
     <hyperlink ref="D27" r:id="rId9" display="X"/>
     <hyperlink ref="D28" r:id="rId10" display="X"/>
     <hyperlink ref="D34" r:id="rId11" display="X"/>
     <hyperlink ref="D35" r:id="rId12" display="X"/>
     <hyperlink ref="D36" r:id="rId13" display="X"/>
     <hyperlink ref="D45" r:id="rId14" display="X"/>
-    <hyperlink ref="D53" r:id="rId15" display="X"/>
-    <hyperlink ref="D60" r:id="rId16" display="X"/>
-    <hyperlink ref="D74" r:id="rId17" display="X"/>
-    <hyperlink ref="D75" r:id="rId18" display="X"/>
-    <hyperlink ref="D81" r:id="rId19" display="X"/>
-    <hyperlink ref="D102" r:id="rId20" display="X"/>
-    <hyperlink ref="D109" r:id="rId21" display="X"/>
+    <hyperlink ref="D46" r:id="rId15" display="X"/>
+    <hyperlink ref="D53" r:id="rId16" display="X"/>
+    <hyperlink ref="D60" r:id="rId17" display="X"/>
+    <hyperlink ref="D67" r:id="rId18" display="X"/>
+    <hyperlink ref="D74" r:id="rId19" display="X"/>
+    <hyperlink ref="D75" r:id="rId20" display="X"/>
+    <hyperlink ref="D81" r:id="rId21" display="X"/>
+    <hyperlink ref="D88" r:id="rId22" display="X"/>
+    <hyperlink ref="D95" r:id="rId23" display="X"/>
+    <hyperlink ref="D102" r:id="rId24" display="X"/>
+    <hyperlink ref="D109" r:id="rId25" display="X"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4969,6 +4916,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>